<commit_message>
Modification dictionnaire de données; Ajout des différentes valeurs pour l'entité user
</commit_message>
<xml_diff>
--- a/01_Conception/Dictionnaire de données.xlsx
+++ b/01_Conception/Dictionnaire de données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfouet/Documents/Git/Github/LIDEM/TP/TP_Symfony_Projet_Photography/01_Conception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE0E0DE-B860-754E-9F54-6C476C30FA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CA6B19-4C69-8B4C-9B55-E54CBC4C53AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{CF490B3E-D7AA-634B-8C7C-B59D837856F2}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,7 +698,9 @@
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
@@ -711,7 +713,9 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>75</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>23</v>
       </c>

</xml_diff>